<commit_message>
Refining number labels and the masterlist.
</commit_message>
<xml_diff>
--- a/datasheets/gen2_masterllist.xlsx
+++ b/datasheets/gen2_masterllist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/warming-SBB/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBFCC92-F161-974B-B724-418A4FB17F86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D32764-93B5-D942-B711-853672A72C2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="24280" windowHeight="16660" xr2:uid="{AEBF1F7C-20FE-134B-832F-8E5E13C6FC57}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="48">
   <si>
     <t>gen2_ID</t>
   </si>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E7CA8A-E8C4-3A4B-B5C5-1E4C1E354B06}">
   <dimension ref="A1:T456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A326" zoomScale="150" zoomScaleNormal="217" workbookViewId="0">
-      <selection activeCell="C337" sqref="C337"/>
+    <sheetView tabSelected="1" topLeftCell="A442" zoomScale="150" zoomScaleNormal="217" workbookViewId="0">
+      <selection activeCell="F449" sqref="F449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -11372,37 +11372,68 @@
       <c r="S342" s="2"/>
     </row>
     <row r="343" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A343" s="2">
-        <f t="shared" ref="A343:A406" si="1">A342+1</f>
-        <v>2329</v>
-      </c>
-      <c r="B343" s="2"/>
-      <c r="C343" s="2"/>
-      <c r="D343" s="2">
-        <v>70</v>
-      </c>
-      <c r="E343" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F343" s="2"/>
-      <c r="G343" s="2"/>
-      <c r="H343" s="2"/>
-      <c r="I343" s="2"/>
-      <c r="J343" s="2"/>
-      <c r="K343" s="2"/>
-      <c r="L343" s="2"/>
-      <c r="M343" s="2"/>
-      <c r="N343" s="2"/>
-      <c r="O343" s="2"/>
-      <c r="P343" s="2"/>
-      <c r="Q343" s="2"/>
-      <c r="R343" s="2"/>
-      <c r="S343" s="2"/>
+      <c r="A343" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B343" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C343" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D343" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E343" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F343" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G343" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H343" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I343" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J343" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K343" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L343" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M343" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N343" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O343" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P343" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q343" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R343" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S343" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="344" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A344" s="2">
-        <f t="shared" si="1"/>
-        <v>2330</v>
+        <f>A342+1</f>
+        <v>2329</v>
       </c>
       <c r="B344" s="2"/>
       <c r="C344" s="2"/>
@@ -11429,8 +11460,8 @@
     </row>
     <row r="345" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A345" s="2">
-        <f t="shared" si="1"/>
-        <v>2331</v>
+        <f t="shared" ref="A345:A408" si="1">A344+1</f>
+        <v>2330</v>
       </c>
       <c r="B345" s="2"/>
       <c r="C345" s="2"/>
@@ -11458,7 +11489,7 @@
     <row r="346" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A346" s="2">
         <f t="shared" si="1"/>
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="B346" s="2"/>
       <c r="C346" s="2"/>
@@ -11486,7 +11517,7 @@
     <row r="347" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A347" s="2">
         <f t="shared" si="1"/>
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="B347" s="2"/>
       <c r="C347" s="2"/>
@@ -11514,7 +11545,7 @@
     <row r="348" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A348" s="2">
         <f t="shared" si="1"/>
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="B348" s="2"/>
       <c r="C348" s="2"/>
@@ -11542,7 +11573,7 @@
     <row r="349" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A349" s="2">
         <f t="shared" si="1"/>
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="B349" s="2"/>
       <c r="C349" s="2"/>
@@ -11570,7 +11601,7 @@
     <row r="350" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A350" s="2">
         <f t="shared" si="1"/>
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="B350" s="2"/>
       <c r="C350" s="2"/>
@@ -11598,7 +11629,7 @@
     <row r="351" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A351" s="2">
         <f t="shared" si="1"/>
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
@@ -11626,7 +11657,7 @@
     <row r="352" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A352" s="2">
         <f t="shared" si="1"/>
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="B352" s="2"/>
       <c r="C352" s="2"/>
@@ -11654,7 +11685,7 @@
     <row r="353" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A353" s="2">
         <f t="shared" si="1"/>
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="B353" s="2"/>
       <c r="C353" s="2"/>
@@ -11682,7 +11713,7 @@
     <row r="354" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A354" s="2">
         <f t="shared" si="1"/>
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="B354" s="2"/>
       <c r="C354" s="2"/>
@@ -11710,7 +11741,7 @@
     <row r="355" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A355" s="2">
         <f t="shared" si="1"/>
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="B355" s="2"/>
       <c r="C355" s="2"/>
@@ -11738,7 +11769,7 @@
     <row r="356" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A356" s="2">
         <f t="shared" si="1"/>
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="B356" s="2"/>
       <c r="C356" s="2"/>
@@ -11766,7 +11797,7 @@
     <row r="357" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A357" s="2">
         <f t="shared" si="1"/>
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="B357" s="2"/>
       <c r="C357" s="2"/>
@@ -11794,7 +11825,7 @@
     <row r="358" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A358" s="2">
         <f t="shared" si="1"/>
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="B358" s="2"/>
       <c r="C358" s="2"/>
@@ -11822,7 +11853,7 @@
     <row r="359" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A359" s="2">
         <f t="shared" si="1"/>
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="B359" s="2"/>
       <c r="C359" s="2"/>
@@ -11850,7 +11881,7 @@
     <row r="360" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A360" s="2">
         <f t="shared" si="1"/>
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="B360" s="2"/>
       <c r="C360" s="2"/>
@@ -11878,7 +11909,7 @@
     <row r="361" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A361" s="2">
         <f t="shared" si="1"/>
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="B361" s="2"/>
       <c r="C361" s="2"/>
@@ -11906,7 +11937,7 @@
     <row r="362" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A362" s="2">
         <f t="shared" si="1"/>
-        <v>2348</v>
+        <v>2347</v>
       </c>
       <c r="B362" s="2"/>
       <c r="C362" s="2"/>
@@ -11934,7 +11965,7 @@
     <row r="363" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A363" s="2">
         <f t="shared" si="1"/>
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="B363" s="2"/>
       <c r="C363" s="2"/>
@@ -11962,7 +11993,7 @@
     <row r="364" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A364" s="2">
         <f t="shared" si="1"/>
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="B364" s="2"/>
       <c r="C364" s="2"/>
@@ -11990,7 +12021,7 @@
     <row r="365" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A365" s="2">
         <f t="shared" si="1"/>
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="B365" s="2"/>
       <c r="C365" s="2"/>
@@ -12018,7 +12049,7 @@
     <row r="366" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A366" s="2">
         <f t="shared" si="1"/>
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="B366" s="2"/>
       <c r="C366" s="2"/>
@@ -12046,7 +12077,7 @@
     <row r="367" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A367" s="2">
         <f t="shared" si="1"/>
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="B367" s="2"/>
       <c r="C367" s="2"/>
@@ -12074,7 +12105,7 @@
     <row r="368" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A368" s="2">
         <f t="shared" si="1"/>
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="B368" s="2"/>
       <c r="C368" s="2"/>
@@ -12102,7 +12133,7 @@
     <row r="369" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A369" s="2">
         <f t="shared" si="1"/>
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="B369" s="2"/>
       <c r="C369" s="2"/>
@@ -12130,7 +12161,7 @@
     <row r="370" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A370" s="2">
         <f t="shared" si="1"/>
-        <v>2356</v>
+        <v>2355</v>
       </c>
       <c r="B370" s="2"/>
       <c r="C370" s="2"/>
@@ -12158,7 +12189,7 @@
     <row r="371" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A371" s="2">
         <f t="shared" si="1"/>
-        <v>2357</v>
+        <v>2356</v>
       </c>
       <c r="B371" s="2"/>
       <c r="C371" s="2"/>
@@ -12186,7 +12217,7 @@
     <row r="372" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A372" s="2">
         <f t="shared" si="1"/>
-        <v>2358</v>
+        <v>2357</v>
       </c>
       <c r="B372" s="2"/>
       <c r="C372" s="2"/>
@@ -12214,7 +12245,7 @@
     <row r="373" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A373" s="2">
         <f t="shared" si="1"/>
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="B373" s="2"/>
       <c r="C373" s="2"/>
@@ -12242,7 +12273,7 @@
     <row r="374" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A374" s="2">
         <f t="shared" si="1"/>
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="B374" s="2"/>
       <c r="C374" s="2"/>
@@ -12270,7 +12301,7 @@
     <row r="375" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A375" s="2">
         <f t="shared" si="1"/>
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="B375" s="2"/>
       <c r="C375" s="2"/>
@@ -12298,7 +12329,7 @@
     <row r="376" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A376" s="2">
         <f t="shared" si="1"/>
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="B376" s="2"/>
       <c r="C376" s="2"/>
@@ -12326,7 +12357,7 @@
     <row r="377" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A377" s="2">
         <f t="shared" si="1"/>
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="B377" s="2"/>
       <c r="C377" s="2"/>
@@ -12354,7 +12385,7 @@
     <row r="378" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A378" s="2">
         <f t="shared" si="1"/>
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="B378" s="2"/>
       <c r="C378" s="2"/>
@@ -12382,7 +12413,7 @@
     <row r="379" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A379" s="2">
         <f t="shared" si="1"/>
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="B379" s="2"/>
       <c r="C379" s="2"/>
@@ -12410,7 +12441,7 @@
     <row r="380" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A380" s="2">
         <f t="shared" si="1"/>
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
@@ -12436,37 +12467,68 @@
       <c r="S380" s="2"/>
     </row>
     <row r="381" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A381" s="2">
-        <f t="shared" si="1"/>
-        <v>2367</v>
-      </c>
-      <c r="B381" s="2"/>
-      <c r="C381" s="2"/>
-      <c r="D381" s="2">
-        <v>70</v>
-      </c>
-      <c r="E381" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F381" s="2"/>
-      <c r="G381" s="2"/>
-      <c r="H381" s="2"/>
-      <c r="I381" s="2"/>
-      <c r="J381" s="2"/>
-      <c r="K381" s="2"/>
-      <c r="L381" s="2"/>
-      <c r="M381" s="2"/>
-      <c r="N381" s="2"/>
-      <c r="O381" s="2"/>
-      <c r="P381" s="2"/>
-      <c r="Q381" s="2"/>
-      <c r="R381" s="2"/>
-      <c r="S381" s="2"/>
+      <c r="A381" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B381" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C381" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D381" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E381" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F381" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G381" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H381" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I381" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J381" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K381" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L381" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M381" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N381" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O381" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P381" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q381" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R381" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S381" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="382" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A382" s="2">
-        <f t="shared" si="1"/>
-        <v>2368</v>
+        <f>A380+1</f>
+        <v>2366</v>
       </c>
       <c r="B382" s="2"/>
       <c r="C382" s="2"/>
@@ -12494,7 +12556,7 @@
     <row r="383" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A383" s="2">
         <f t="shared" si="1"/>
-        <v>2369</v>
+        <v>2367</v>
       </c>
       <c r="B383" s="2"/>
       <c r="C383" s="2"/>
@@ -12522,7 +12584,7 @@
     <row r="384" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A384" s="2">
         <f t="shared" si="1"/>
-        <v>2370</v>
+        <v>2368</v>
       </c>
       <c r="B384" s="2"/>
       <c r="C384" s="2"/>
@@ -12550,7 +12612,7 @@
     <row r="385" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A385" s="2">
         <f t="shared" si="1"/>
-        <v>2371</v>
+        <v>2369</v>
       </c>
       <c r="B385" s="2"/>
       <c r="C385" s="2"/>
@@ -12578,7 +12640,7 @@
     <row r="386" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A386" s="2">
         <f t="shared" si="1"/>
-        <v>2372</v>
+        <v>2370</v>
       </c>
       <c r="B386" s="2"/>
       <c r="C386" s="2"/>
@@ -12606,7 +12668,7 @@
     <row r="387" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A387" s="2">
         <f t="shared" si="1"/>
-        <v>2373</v>
+        <v>2371</v>
       </c>
       <c r="B387" s="2"/>
       <c r="C387" s="2"/>
@@ -12634,7 +12696,7 @@
     <row r="388" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A388" s="2">
         <f t="shared" si="1"/>
-        <v>2374</v>
+        <v>2372</v>
       </c>
       <c r="B388" s="2"/>
       <c r="C388" s="2"/>
@@ -12662,7 +12724,7 @@
     <row r="389" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A389" s="2">
         <f t="shared" si="1"/>
-        <v>2375</v>
+        <v>2373</v>
       </c>
       <c r="B389" s="2"/>
       <c r="C389" s="2"/>
@@ -12690,7 +12752,7 @@
     <row r="390" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A390" s="2">
         <f t="shared" si="1"/>
-        <v>2376</v>
+        <v>2374</v>
       </c>
       <c r="B390" s="2"/>
       <c r="C390" s="2"/>
@@ -12718,7 +12780,7 @@
     <row r="391" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A391" s="2">
         <f t="shared" si="1"/>
-        <v>2377</v>
+        <v>2375</v>
       </c>
       <c r="B391" s="2"/>
       <c r="C391" s="2"/>
@@ -12746,7 +12808,7 @@
     <row r="392" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A392" s="2">
         <f t="shared" si="1"/>
-        <v>2378</v>
+        <v>2376</v>
       </c>
       <c r="B392" s="2"/>
       <c r="C392" s="2"/>
@@ -12774,7 +12836,7 @@
     <row r="393" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A393" s="2">
         <f t="shared" si="1"/>
-        <v>2379</v>
+        <v>2377</v>
       </c>
       <c r="B393" s="2"/>
       <c r="C393" s="2"/>
@@ -12802,7 +12864,7 @@
     <row r="394" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A394" s="2">
         <f t="shared" si="1"/>
-        <v>2380</v>
+        <v>2378</v>
       </c>
       <c r="B394" s="2"/>
       <c r="C394" s="2"/>
@@ -12830,7 +12892,7 @@
     <row r="395" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A395" s="2">
         <f t="shared" si="1"/>
-        <v>2381</v>
+        <v>2379</v>
       </c>
       <c r="B395" s="2"/>
       <c r="C395" s="2"/>
@@ -12858,7 +12920,7 @@
     <row r="396" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A396" s="2">
         <f t="shared" si="1"/>
-        <v>2382</v>
+        <v>2380</v>
       </c>
       <c r="B396" s="2"/>
       <c r="C396" s="2"/>
@@ -12886,7 +12948,7 @@
     <row r="397" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A397" s="2">
         <f t="shared" si="1"/>
-        <v>2383</v>
+        <v>2381</v>
       </c>
       <c r="B397" s="2"/>
       <c r="C397" s="2"/>
@@ -12914,7 +12976,7 @@
     <row r="398" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A398" s="2">
         <f t="shared" si="1"/>
-        <v>2384</v>
+        <v>2382</v>
       </c>
       <c r="B398" s="2"/>
       <c r="C398" s="2"/>
@@ -12942,7 +13004,7 @@
     <row r="399" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A399" s="2">
         <f t="shared" si="1"/>
-        <v>2385</v>
+        <v>2383</v>
       </c>
       <c r="B399" s="2"/>
       <c r="C399" s="2"/>
@@ -12970,7 +13032,7 @@
     <row r="400" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A400" s="2">
         <f t="shared" si="1"/>
-        <v>2386</v>
+        <v>2384</v>
       </c>
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
@@ -12998,7 +13060,7 @@
     <row r="401" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A401" s="2">
         <f t="shared" si="1"/>
-        <v>2387</v>
+        <v>2385</v>
       </c>
       <c r="B401" s="2"/>
       <c r="C401" s="2"/>
@@ -13026,7 +13088,7 @@
     <row r="402" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A402" s="2">
         <f t="shared" si="1"/>
-        <v>2388</v>
+        <v>2386</v>
       </c>
       <c r="B402" s="2"/>
       <c r="C402" s="2"/>
@@ -13054,7 +13116,7 @@
     <row r="403" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A403" s="2">
         <f t="shared" si="1"/>
-        <v>2389</v>
+        <v>2387</v>
       </c>
       <c r="B403" s="2"/>
       <c r="C403" s="2"/>
@@ -13082,7 +13144,7 @@
     <row r="404" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A404" s="2">
         <f t="shared" si="1"/>
-        <v>2390</v>
+        <v>2388</v>
       </c>
       <c r="B404" s="2"/>
       <c r="C404" s="2"/>
@@ -13110,7 +13172,7 @@
     <row r="405" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A405" s="2">
         <f t="shared" si="1"/>
-        <v>2391</v>
+        <v>2389</v>
       </c>
       <c r="B405" s="2"/>
       <c r="C405" s="2"/>
@@ -13138,7 +13200,7 @@
     <row r="406" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A406" s="2">
         <f t="shared" si="1"/>
-        <v>2392</v>
+        <v>2390</v>
       </c>
       <c r="B406" s="2"/>
       <c r="C406" s="2"/>
@@ -13165,8 +13227,8 @@
     </row>
     <row r="407" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A407" s="2">
-        <f t="shared" ref="A407:A419" si="2">A406+1</f>
-        <v>2393</v>
+        <f t="shared" si="1"/>
+        <v>2391</v>
       </c>
       <c r="B407" s="2"/>
       <c r="C407" s="2"/>
@@ -13193,8 +13255,8 @@
     </row>
     <row r="408" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A408" s="2">
-        <f t="shared" si="2"/>
-        <v>2394</v>
+        <f t="shared" si="1"/>
+        <v>2392</v>
       </c>
       <c r="B408" s="2"/>
       <c r="C408" s="2"/>
@@ -13221,8 +13283,8 @@
     </row>
     <row r="409" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A409" s="2">
-        <f t="shared" si="2"/>
-        <v>2395</v>
+        <f t="shared" ref="A409:A422" si="2">A408+1</f>
+        <v>2393</v>
       </c>
       <c r="B409" s="2"/>
       <c r="C409" s="2"/>
@@ -13250,7 +13312,7 @@
     <row r="410" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A410" s="2">
         <f t="shared" si="2"/>
-        <v>2396</v>
+        <v>2394</v>
       </c>
       <c r="B410" s="2"/>
       <c r="C410" s="2"/>
@@ -13278,7 +13340,7 @@
     <row r="411" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A411" s="2">
         <f t="shared" si="2"/>
-        <v>2397</v>
+        <v>2395</v>
       </c>
       <c r="B411" s="2"/>
       <c r="C411" s="2"/>
@@ -13306,7 +13368,7 @@
     <row r="412" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A412" s="2">
         <f t="shared" si="2"/>
-        <v>2398</v>
+        <v>2396</v>
       </c>
       <c r="B412" s="2"/>
       <c r="C412" s="2"/>
@@ -13334,7 +13396,7 @@
     <row r="413" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A413" s="2">
         <f t="shared" si="2"/>
-        <v>2399</v>
+        <v>2397</v>
       </c>
       <c r="B413" s="2"/>
       <c r="C413" s="2"/>
@@ -13362,7 +13424,7 @@
     <row r="414" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A414" s="2">
         <f t="shared" si="2"/>
-        <v>2400</v>
+        <v>2398</v>
       </c>
       <c r="B414" s="2"/>
       <c r="C414" s="2"/>
@@ -13390,7 +13452,7 @@
     <row r="415" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A415" s="2">
         <f t="shared" si="2"/>
-        <v>2401</v>
+        <v>2399</v>
       </c>
       <c r="B415" s="2"/>
       <c r="C415" s="2"/>
@@ -13418,7 +13480,7 @@
     <row r="416" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A416" s="2">
         <f t="shared" si="2"/>
-        <v>2402</v>
+        <v>2400</v>
       </c>
       <c r="B416" s="2"/>
       <c r="C416" s="2"/>
@@ -13446,7 +13508,7 @@
     <row r="417" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A417" s="2">
         <f t="shared" si="2"/>
-        <v>2403</v>
+        <v>2401</v>
       </c>
       <c r="B417" s="2"/>
       <c r="C417" s="2"/>
@@ -13474,7 +13536,7 @@
     <row r="418" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A418" s="2">
         <f t="shared" si="2"/>
-        <v>2404</v>
+        <v>2402</v>
       </c>
       <c r="B418" s="2"/>
       <c r="C418" s="2"/>
@@ -13500,37 +13562,68 @@
       <c r="S418" s="2"/>
     </row>
     <row r="419" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A419" s="2">
-        <f t="shared" si="2"/>
-        <v>2405</v>
-      </c>
-      <c r="B419" s="2"/>
-      <c r="C419" s="2"/>
-      <c r="D419" s="2">
-        <v>70</v>
-      </c>
-      <c r="E419" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F419" s="2"/>
-      <c r="G419" s="2"/>
-      <c r="H419" s="2"/>
-      <c r="I419" s="2"/>
-      <c r="J419" s="2"/>
-      <c r="K419" s="2"/>
-      <c r="L419" s="2"/>
-      <c r="M419" s="2"/>
-      <c r="N419" s="2"/>
-      <c r="O419" s="2"/>
-      <c r="P419" s="2"/>
-      <c r="Q419" s="2"/>
-      <c r="R419" s="2"/>
-      <c r="S419" s="2"/>
+      <c r="A419" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B419" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C419" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D419" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E419" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F419" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G419" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H419" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I419" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J419" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K419" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L419" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M419" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N419" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O419" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P419" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q419" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R419" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S419" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="420" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A420" s="2">
-        <f t="shared" ref="A420:A434" si="3">A419+1</f>
-        <v>2406</v>
+        <f>A418+1</f>
+        <v>2403</v>
       </c>
       <c r="B420" s="2"/>
       <c r="C420" s="2"/>
@@ -13557,8 +13650,8 @@
     </row>
     <row r="421" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A421" s="2">
-        <f t="shared" si="3"/>
-        <v>2407</v>
+        <f t="shared" si="2"/>
+        <v>2404</v>
       </c>
       <c r="B421" s="2"/>
       <c r="C421" s="2"/>
@@ -13585,8 +13678,8 @@
     </row>
     <row r="422" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A422" s="2">
-        <f t="shared" si="3"/>
-        <v>2408</v>
+        <f t="shared" si="2"/>
+        <v>2405</v>
       </c>
       <c r="B422" s="2"/>
       <c r="C422" s="2"/>
@@ -13613,8 +13706,8 @@
     </row>
     <row r="423" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A423" s="2">
-        <f t="shared" si="3"/>
-        <v>2409</v>
+        <f t="shared" ref="A423:A437" si="3">A422+1</f>
+        <v>2406</v>
       </c>
       <c r="B423" s="2"/>
       <c r="C423" s="2"/>
@@ -13642,7 +13735,7 @@
     <row r="424" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A424" s="2">
         <f t="shared" si="3"/>
-        <v>2410</v>
+        <v>2407</v>
       </c>
       <c r="B424" s="2"/>
       <c r="C424" s="2"/>
@@ -13670,7 +13763,7 @@
     <row r="425" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A425" s="2">
         <f t="shared" si="3"/>
-        <v>2411</v>
+        <v>2408</v>
       </c>
       <c r="B425" s="2"/>
       <c r="C425" s="2"/>
@@ -13698,7 +13791,7 @@
     <row r="426" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A426" s="2">
         <f t="shared" si="3"/>
-        <v>2412</v>
+        <v>2409</v>
       </c>
       <c r="B426" s="2"/>
       <c r="C426" s="2"/>
@@ -13726,7 +13819,7 @@
     <row r="427" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A427" s="2">
         <f t="shared" si="3"/>
-        <v>2413</v>
+        <v>2410</v>
       </c>
       <c r="B427" s="2"/>
       <c r="C427" s="2"/>
@@ -13754,7 +13847,7 @@
     <row r="428" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A428" s="2">
         <f t="shared" si="3"/>
-        <v>2414</v>
+        <v>2411</v>
       </c>
       <c r="B428" s="2"/>
       <c r="C428" s="2"/>
@@ -13782,7 +13875,7 @@
     <row r="429" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A429" s="2">
         <f t="shared" si="3"/>
-        <v>2415</v>
+        <v>2412</v>
       </c>
       <c r="B429" s="2"/>
       <c r="C429" s="2"/>
@@ -13810,7 +13903,7 @@
     <row r="430" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A430" s="2">
         <f t="shared" si="3"/>
-        <v>2416</v>
+        <v>2413</v>
       </c>
       <c r="B430" s="2"/>
       <c r="C430" s="2"/>
@@ -13838,7 +13931,7 @@
     <row r="431" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A431" s="2">
         <f t="shared" si="3"/>
-        <v>2417</v>
+        <v>2414</v>
       </c>
       <c r="B431" s="2"/>
       <c r="C431" s="2"/>
@@ -13866,7 +13959,7 @@
     <row r="432" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A432" s="2">
         <f t="shared" si="3"/>
-        <v>2418</v>
+        <v>2415</v>
       </c>
       <c r="B432" s="2"/>
       <c r="C432" s="2"/>
@@ -13894,7 +13987,7 @@
     <row r="433" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A433" s="2">
         <f t="shared" si="3"/>
-        <v>2419</v>
+        <v>2416</v>
       </c>
       <c r="B433" s="2"/>
       <c r="C433" s="2"/>
@@ -13922,7 +14015,7 @@
     <row r="434" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A434" s="2">
         <f t="shared" si="3"/>
-        <v>2420</v>
+        <v>2417</v>
       </c>
       <c r="B434" s="2"/>
       <c r="C434" s="2"/>
@@ -13949,8 +14042,8 @@
     </row>
     <row r="435" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A435" s="2">
-        <f t="shared" ref="A435:A456" si="4">A434+1</f>
-        <v>2421</v>
+        <f t="shared" si="3"/>
+        <v>2418</v>
       </c>
       <c r="B435" s="2"/>
       <c r="C435" s="2"/>
@@ -13977,8 +14070,8 @@
     </row>
     <row r="436" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A436" s="2">
-        <f t="shared" si="4"/>
-        <v>2422</v>
+        <f t="shared" si="3"/>
+        <v>2419</v>
       </c>
       <c r="B436" s="2"/>
       <c r="C436" s="2"/>
@@ -14005,8 +14098,8 @@
     </row>
     <row r="437" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A437" s="2">
-        <f t="shared" si="4"/>
-        <v>2423</v>
+        <f t="shared" si="3"/>
+        <v>2420</v>
       </c>
       <c r="B437" s="2"/>
       <c r="C437" s="2"/>
@@ -14033,8 +14126,8 @@
     </row>
     <row r="438" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A438" s="2">
-        <f t="shared" si="4"/>
-        <v>2424</v>
+        <f t="shared" ref="A438:A456" si="4">A437+1</f>
+        <v>2421</v>
       </c>
       <c r="B438" s="2"/>
       <c r="C438" s="2"/>
@@ -14062,7 +14155,7 @@
     <row r="439" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A439" s="2">
         <f t="shared" si="4"/>
-        <v>2425</v>
+        <v>2422</v>
       </c>
       <c r="B439" s="2"/>
       <c r="C439" s="2"/>
@@ -14090,7 +14183,7 @@
     <row r="440" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A440" s="2">
         <f t="shared" si="4"/>
-        <v>2426</v>
+        <v>2423</v>
       </c>
       <c r="B440" s="2"/>
       <c r="C440" s="2"/>
@@ -14118,7 +14211,7 @@
     <row r="441" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A441" s="2">
         <f t="shared" si="4"/>
-        <v>2427</v>
+        <v>2424</v>
       </c>
       <c r="B441" s="2"/>
       <c r="C441" s="2"/>
@@ -14146,7 +14239,7 @@
     <row r="442" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A442" s="2">
         <f t="shared" si="4"/>
-        <v>2428</v>
+        <v>2425</v>
       </c>
       <c r="B442" s="2"/>
       <c r="C442" s="2"/>
@@ -14174,7 +14267,7 @@
     <row r="443" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A443" s="2">
         <f t="shared" si="4"/>
-        <v>2429</v>
+        <v>2426</v>
       </c>
       <c r="B443" s="2"/>
       <c r="C443" s="2"/>
@@ -14202,7 +14295,7 @@
     <row r="444" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A444" s="2">
         <f t="shared" si="4"/>
-        <v>2430</v>
+        <v>2427</v>
       </c>
       <c r="B444" s="2"/>
       <c r="C444" s="2"/>
@@ -14230,7 +14323,7 @@
     <row r="445" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A445" s="2">
         <f t="shared" si="4"/>
-        <v>2431</v>
+        <v>2428</v>
       </c>
       <c r="B445" s="2"/>
       <c r="C445" s="2"/>
@@ -14258,7 +14351,7 @@
     <row r="446" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A446" s="2">
         <f t="shared" si="4"/>
-        <v>2432</v>
+        <v>2429</v>
       </c>
       <c r="B446" s="2"/>
       <c r="C446" s="2"/>
@@ -14286,7 +14379,7 @@
     <row r="447" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A447" s="2">
         <f t="shared" si="4"/>
-        <v>2433</v>
+        <v>2430</v>
       </c>
       <c r="B447" s="2"/>
       <c r="C447" s="2"/>
@@ -14314,7 +14407,7 @@
     <row r="448" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A448" s="2">
         <f t="shared" si="4"/>
-        <v>2434</v>
+        <v>2431</v>
       </c>
       <c r="B448" s="2"/>
       <c r="C448" s="2"/>
@@ -14342,7 +14435,7 @@
     <row r="449" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A449" s="2">
         <f t="shared" si="4"/>
-        <v>2435</v>
+        <v>2432</v>
       </c>
       <c r="B449" s="2"/>
       <c r="C449" s="2"/>
@@ -14370,7 +14463,7 @@
     <row r="450" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A450" s="2">
         <f t="shared" si="4"/>
-        <v>2436</v>
+        <v>2433</v>
       </c>
       <c r="B450" s="2"/>
       <c r="C450" s="2"/>
@@ -14398,7 +14491,7 @@
     <row r="451" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A451" s="2">
         <f t="shared" si="4"/>
-        <v>2437</v>
+        <v>2434</v>
       </c>
       <c r="B451" s="2"/>
       <c r="C451" s="2"/>
@@ -14426,7 +14519,7 @@
     <row r="452" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A452" s="2">
         <f t="shared" si="4"/>
-        <v>2438</v>
+        <v>2435</v>
       </c>
       <c r="B452" s="2"/>
       <c r="C452" s="2"/>
@@ -14454,7 +14547,7 @@
     <row r="453" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A453" s="2">
         <f t="shared" si="4"/>
-        <v>2439</v>
+        <v>2436</v>
       </c>
       <c r="B453" s="2"/>
       <c r="C453" s="2"/>
@@ -14482,7 +14575,7 @@
     <row r="454" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A454" s="2">
         <f t="shared" si="4"/>
-        <v>2440</v>
+        <v>2437</v>
       </c>
       <c r="B454" s="2"/>
       <c r="C454" s="2"/>
@@ -14510,7 +14603,7 @@
     <row r="455" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A455" s="2">
         <f t="shared" si="4"/>
-        <v>2441</v>
+        <v>2438</v>
       </c>
       <c r="B455" s="2"/>
       <c r="C455" s="2"/>
@@ -14538,7 +14631,7 @@
     <row r="456" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A456" s="2">
         <f t="shared" si="4"/>
-        <v>2442</v>
+        <v>2439</v>
       </c>
       <c r="B456" s="2"/>
       <c r="C456" s="2"/>

</xml_diff>